<commit_message>
Money S4 almost done
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>AA1</t>
+  </si>
+  <si>
+    <t>ChangedOn</t>
   </si>
 </sst>
 </file>
@@ -192,7 +198,10 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -240,12 +249,13 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabulka5711" displayName="Tabulka5711" ref="A15:C19" totalsRowShown="0">
-  <autoFilter ref="A15:C19"/>
-  <tableColumns count="3">
-    <tableColumn id="3" name="ExternalId" dataDxfId="2"/>
-    <tableColumn id="4" name="AdapterId" dataDxfId="1"/>
-    <tableColumn id="5" name="AccountId" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabulka5711" displayName="Tabulka5711" ref="A15:D19" totalsRowShown="0">
+  <autoFilter ref="A15:D19"/>
+  <tableColumns count="4">
+    <tableColumn id="3" name="ExternalId" dataDxfId="3"/>
+    <tableColumn id="4" name="AdapterId" dataDxfId="2"/>
+    <tableColumn id="5" name="AccountId" dataDxfId="1"/>
+    <tableColumn id="6" name="ChangedOn" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -305,16 +315,16 @@
   <autoFilter ref="A15:E19"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Title" dataDxfId="6">
+    <tableColumn id="2" name="Title" dataDxfId="7">
       <calculatedColumnFormula>C3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ExternalId" dataDxfId="4">
+    <tableColumn id="3" name="ExternalId" dataDxfId="5">
       <calculatedColumnFormula>E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="AdapterId" dataDxfId="5">
+    <tableColumn id="4" name="AdapterId" dataDxfId="6">
       <calculatedColumnFormula>A1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="AccountId" dataDxfId="3">
+    <tableColumn id="5" name="AccountId" dataDxfId="4">
       <calculatedColumnFormula>A9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -323,26 +333,28 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabulka18" displayName="Tabulka18" ref="A2:D5" totalsRowShown="0">
-  <autoFilter ref="A2:D5"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabulka18" displayName="Tabulka18" ref="A2:E5" totalsRowShown="0">
+  <autoFilter ref="A2:E5"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Title"/>
     <tableColumn id="3" name="AccountId"/>
     <tableColumn id="4" name="ExternalId"/>
+    <tableColumn id="5" name="AdapterId"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabulka29" displayName="Tabulka29" ref="F2:I5" totalsRowShown="0">
-  <autoFilter ref="F2:I5"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabulka29" displayName="Tabulka29" ref="G2:K5" totalsRowShown="0">
+  <autoFilter ref="G2:K5"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Title"/>
     <tableColumn id="3" name="AccountId"/>
     <tableColumn id="4" name="ExternalId"/>
+    <tableColumn id="5" name="AdapterId"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -983,10 +995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,21 +1006,22 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1021,20 +1034,26 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
       <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1045,9 +1064,15 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1057,11 +1082,17 @@
       <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="E4">
+        <v>1</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1071,13 +1102,16 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1091,12 +1125,26 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1106,20 +1154,45 @@
       <c r="C15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
       <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
       <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
       <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>